<commit_message>
add some concept tags
</commit_message>
<xml_diff>
--- a/extra/vcdExtra-datasets.xlsx
+++ b/extra/vcdExtra-datasets.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Projects\vcdExtra\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{29AE0CDD-8A7A-4038-A8F3-93D5B8F4EE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FE2CF6-5CB9-4270-BD4C-26B8901F3579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vcdExtra-datasets" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="146">
   <si>
     <t>Item</t>
   </si>
@@ -437,12 +437,33 @@
   </si>
   <si>
     <t>glm; poisson</t>
+  </si>
+  <si>
+    <t>one-way</t>
+  </si>
+  <si>
+    <t>loglinear;multinomial;zeros</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>glm</t>
+  </si>
+  <si>
+    <t>loglinear</t>
+  </si>
+  <si>
+    <t>glm;logistic</t>
+  </si>
+  <si>
+    <t>loglinear;logit;2x2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1276,11 +1297,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,6 +1344,9 @@
       <c r="E2" t="s">
         <v>7</v>
       </c>
+      <c r="F2" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1380,6 +1404,9 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
+      <c r="F5" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1417,6 +1444,9 @@
       <c r="E7" t="s">
         <v>21</v>
       </c>
+      <c r="F7" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1494,6 +1524,9 @@
       <c r="E11" t="s">
         <v>32</v>
       </c>
+      <c r="F11" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1511,6 +1544,9 @@
       <c r="E12" t="s">
         <v>35</v>
       </c>
+      <c r="F12" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1528,6 +1564,9 @@
       <c r="E13">
         <v>15</v>
       </c>
+      <c r="F13" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1545,6 +1584,9 @@
       <c r="E14" t="s">
         <v>40</v>
       </c>
+      <c r="F14" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1562,6 +1604,9 @@
       <c r="E15" t="s">
         <v>43</v>
       </c>
+      <c r="F15" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1852,7 +1897,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1869,7 +1914,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1886,7 +1931,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1903,7 +1948,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1920,7 +1965,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1937,7 +1982,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1953,8 +1998,11 @@
       <c r="E38" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1971,7 +2019,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1988,7 +2036,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2005,7 +2053,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2022,7 +2070,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2039,7 +2087,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2056,7 +2104,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
prep NEWS, cran-comments for release
</commit_message>
<xml_diff>
--- a/extra/vcdExtra-datasets.xlsx
+++ b/extra/vcdExtra-datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Projects\vcdExtra\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FE2CF6-5CB9-4270-BD4C-26B8901F3579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978FB3DD-DD4E-4FEF-8E7F-ABEC2C123D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vcdExtra-datasets" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="147">
   <si>
     <t>Item</t>
   </si>
@@ -458,6 +458,9 @@
   </si>
   <si>
     <t>loglinear;logit;2x2</t>
+  </si>
+  <si>
+    <t>square;mobility;reorder</t>
   </si>
 </sst>
 </file>
@@ -1300,8 +1303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1625,7 +1628,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1642,7 +1645,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1659,7 +1662,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1676,7 +1679,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1693,7 +1696,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1710,7 +1713,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1727,7 +1730,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1743,8 +1746,11 @@
       <c r="E23" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1761,7 +1767,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1778,7 +1784,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1795,7 +1801,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1812,7 +1818,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1829,7 +1835,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1846,7 +1852,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1880,7 +1886,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
classify datasets with \concept{}
</commit_message>
<xml_diff>
--- a/extra/vcdExtra-datasets.xlsx
+++ b/extra/vcdExtra-datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Projects\vcdExtra\extra\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{978FB3DD-DD4E-4FEF-8E7F-ABEC2C123D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{362ACEC9-72D3-4A19-B489-0DEEFF959EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="vcdExtra-datasets" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="162">
   <si>
     <t>Item</t>
   </si>
@@ -424,9 +424,6 @@
     <t>loglinear; glm; logistic</t>
   </si>
   <si>
-    <t>loglinear; homogeneity</t>
-  </si>
-  <si>
     <t>reorder; ca</t>
   </si>
   <si>
@@ -461,6 +458,54 @@
   </si>
   <si>
     <t>square;mobility;reorder</t>
+  </si>
+  <si>
+    <t>lm</t>
+  </si>
+  <si>
+    <t>ca;glm;ordinal</t>
+  </si>
+  <si>
+    <t>oddsratio</t>
+  </si>
+  <si>
+    <t>binomial</t>
+  </si>
+  <si>
+    <t>ca;ordinal</t>
+  </si>
+  <si>
+    <t>ordinal</t>
+  </si>
+  <si>
+    <t>square;mobility;ordinal</t>
+  </si>
+  <si>
+    <t>2x2</t>
+  </si>
+  <si>
+    <t>ca;reorder</t>
+  </si>
+  <si>
+    <t>logistic;glm</t>
+  </si>
+  <si>
+    <t>loglinear;ordinal</t>
+  </si>
+  <si>
+    <t>agree;ordinal</t>
+  </si>
+  <si>
+    <t>glm;zeros</t>
+  </si>
+  <si>
+    <t>loglinear;logistic</t>
+  </si>
+  <si>
+    <t>loglinear;zeros</t>
+  </si>
+  <si>
+    <t>2x2;loglinear; homogeneity;odds ratio</t>
   </si>
 </sst>
 </file>
@@ -1301,830 +1346,782 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="44" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17" customWidth="1"/>
+    <col min="2" max="2" width="44" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>43</v>
+      </c>
+      <c r="E15" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E23" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" t="s">
+        <v>73</v>
+      </c>
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
         <v>6</v>
       </c>
-      <c r="E6" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>79</v>
+      </c>
+      <c r="B28" t="s">
+        <v>80</v>
+      </c>
+      <c r="C28" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E31" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>91</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>94</v>
+      </c>
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+      <c r="C33" t="s">
+        <v>55</v>
+      </c>
+      <c r="D33" t="s">
+        <v>93</v>
+      </c>
+      <c r="E33" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34" t="s">
+        <v>98</v>
+      </c>
+      <c r="E34" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" t="s">
+        <v>10</v>
+      </c>
+      <c r="D35" t="s">
+        <v>101</v>
+      </c>
+      <c r="E35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" t="s">
+        <v>6</v>
+      </c>
+      <c r="D36" t="s">
+        <v>104</v>
+      </c>
+      <c r="E36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D37" t="s">
+        <v>107</v>
+      </c>
+      <c r="E37" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" t="s">
+        <v>109</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" t="s">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B39" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
-        <v>40</v>
-      </c>
-      <c r="F14" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" t="s">
-        <v>55</v>
-      </c>
-      <c r="E19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>64</v>
-      </c>
-      <c r="D22" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>66</v>
-      </c>
-      <c r="C23" t="s">
-        <v>67</v>
-      </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24" t="s">
-        <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" t="s">
-        <v>55</v>
-      </c>
-      <c r="E24" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26" t="s">
-        <v>74</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27" t="s">
-        <v>77</v>
-      </c>
-      <c r="C27" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E27" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E28" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" t="s">
-        <v>82</v>
-      </c>
-      <c r="C29" t="s">
-        <v>83</v>
-      </c>
-      <c r="D29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
-      <c r="C30" t="s">
-        <v>86</v>
-      </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-      <c r="E30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" t="s">
-        <v>88</v>
-      </c>
-      <c r="C31" t="s">
-        <v>89</v>
-      </c>
-      <c r="D31" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32" t="s">
-        <v>92</v>
-      </c>
-      <c r="D32" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" t="s">
-        <v>94</v>
-      </c>
-      <c r="C33" t="s">
-        <v>95</v>
-      </c>
-      <c r="D33" t="s">
-        <v>55</v>
-      </c>
-      <c r="E33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
-        <v>96</v>
-      </c>
-      <c r="C34" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" t="s">
-        <v>10</v>
-      </c>
-      <c r="E34" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" t="s">
-        <v>99</v>
-      </c>
-      <c r="C35" t="s">
-        <v>100</v>
-      </c>
-      <c r="D35" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36" t="s">
-        <v>102</v>
-      </c>
-      <c r="C36" t="s">
-        <v>103</v>
-      </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" t="s">
-        <v>106</v>
-      </c>
-      <c r="D37" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38" t="s">
-        <v>108</v>
-      </c>
-      <c r="C38" t="s">
-        <v>109</v>
-      </c>
-      <c r="D38" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" t="s">
-        <v>110</v>
-      </c>
-      <c r="F38" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>111</v>
-      </c>
-      <c r="C39" t="s">
-        <v>112</v>
-      </c>
-      <c r="D39" t="s">
-        <v>55</v>
-      </c>
-      <c r="E39" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>114</v>
       </c>
       <c r="B40" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C40" t="s">
-        <v>115</v>
+        <v>10</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
+        <v>116</v>
       </c>
       <c r="E40" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>117</v>
       </c>
       <c r="B41" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C41" t="s">
-        <v>118</v>
+        <v>10</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
+        <v>119</v>
       </c>
       <c r="E41" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>120</v>
       </c>
       <c r="B42" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
-        <v>121</v>
+        <v>10</v>
       </c>
       <c r="D42" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="E42" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>123</v>
       </c>
       <c r="B43" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C43" t="s">
-        <v>124</v>
+        <v>10</v>
       </c>
       <c r="D43" t="s">
-        <v>10</v>
+        <v>125</v>
       </c>
       <c r="E43" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>126</v>
       </c>
       <c r="B44" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C44" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
+        <v>128</v>
       </c>
       <c r="E44" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>129</v>
       </c>
       <c r="B45" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C45" t="s">
-        <v>130</v>
+        <v>10</v>
       </c>
       <c r="D45" t="s">
-        <v>10</v>
+        <v>131</v>
       </c>
       <c r="E45" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>